<commit_message>
update version to v0.4 add ForEachCommand
</commit_message>
<xml_diff>
--- a/src/test/resources/echo/echo.xlsx
+++ b/src/test/resources/echo/echo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\src\test\resources\echo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C16D15-38CB-4373-9B6A-EF0F227363E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D12D17-465D-4FF2-9485-AD6DA578E839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,16 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>TestCase</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>admin</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>echo</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -45,6 +41,18 @@
   </si>
   <si>
     <t>{"file":"C:\\Users\\xihu_\\Desktop\\2.json"}</t>
+  </si>
+  <si>
+    <t>{"target":"admin"}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pause</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{"target":2000}</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -68,13 +76,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color indexed="8"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
@@ -91,6 +92,13 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0451A5"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
     </font>
@@ -136,13 +144,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
@@ -465,53 +473,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5">
+        <v>2000</v>
+      </c>
+      <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update javascript engine. update test case.
</commit_message>
<xml_diff>
--- a/src/test/resources/echo/echo.xlsx
+++ b/src/test/resources/echo/echo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\src\test\resources\echo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\github\auto-test\src\test\resources\echo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F45833-6A86-4AD5-AD66-F1A0460EA6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0A3D28-7AAF-4549-AF8B-447063664B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>readProperties</t>
-  </si>
-  <si>
     <t>{"target":"admin"}</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -47,9 +44,6 @@
   <si>
     <t>{"target":2000}</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{"value":"download/2.json"}</t>
   </si>
   <si>
     <r>
@@ -75,6 +69,14 @@
       </rPr>
       <t>":"json"}</t>
     </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>setProperty</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{"name":"hugang","admin":"administrator"}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -296,31 +298,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -651,25 +653,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.25" style="1"/>
+    <col min="5" max="5" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>1</v>
@@ -678,16 +682,16 @@
         <v>1</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -698,20 +702,20 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.45">
       <c r="A3" s="6">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>